<commit_message>
"Log all coming smss and test project on real condition"
</commit_message>
<xml_diff>
--- a/app/Data/data.xlsx
+++ b/app/Data/data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t xml:space="preserve">row</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t xml:space="preserve">jj7654321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DD1245</t>
   </si>
   <si>
     <t xml:space="preserve">faulty</t>
@@ -182,10 +191,10 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="38.2"/>
@@ -273,10 +282,44 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F5" s="1"/>
+      <c r="A5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>44450</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F6" s="1"/>
+      <c r="A6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>41092</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -297,29 +340,32 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>